<commit_message>
Add some plot module in the DCAE project.
</commit_message>
<xml_diff>
--- a/DCAE_diagnosis/experiment1.xlsx
+++ b/DCAE_diagnosis/experiment1.xlsx
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD26" sqref="AD26:AK28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Modify the plot_module of "DCAE_diagnosis"
</commit_message>
<xml_diff>
--- a/DCAE_diagnosis/experiment1.xlsx
+++ b/DCAE_diagnosis/experiment1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>系数</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,6 +138,14 @@
   </si>
   <si>
     <t>DCAE-1D+SDAE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDCNN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DCAE-1D+ WDCNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -540,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP38"/>
+  <dimension ref="A1:AR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -555,19 +563,21 @@
     <col min="8" max="12" width="23" style="1" customWidth="1"/>
     <col min="13" max="13" width="22.75" style="1" customWidth="1"/>
     <col min="14" max="15" width="14.625" style="1" customWidth="1"/>
-    <col min="16" max="21" width="9" style="1"/>
-    <col min="22" max="22" width="8.75" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.625" style="1" customWidth="1"/>
-    <col min="24" max="26" width="9" style="1"/>
-    <col min="27" max="27" width="10.625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="1"/>
-    <col min="29" max="29" width="15.25" style="1" customWidth="1"/>
-    <col min="30" max="30" width="21.125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="25.375" customWidth="1"/>
-    <col min="32" max="16384" width="9" style="1"/>
+    <col min="16" max="16" width="15.375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.625" style="1" customWidth="1"/>
+    <col min="18" max="23" width="9" style="1"/>
+    <col min="24" max="24" width="8.75" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.625" style="1" customWidth="1"/>
+    <col min="26" max="28" width="9" style="1"/>
+    <col min="29" max="29" width="10.625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="9" style="1"/>
+    <col min="31" max="31" width="15.25" style="1" customWidth="1"/>
+    <col min="32" max="32" width="21.125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="25.375" customWidth="1"/>
+    <col min="34" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,82 +624,88 @@
         <v>29</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AK1" s="1">
         <v>86.05</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AL1" s="1">
         <v>90.61</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AN1" s="1">
         <v>96.08</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AO1" s="1">
         <v>99.1</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AP1" s="1">
         <v>99.72</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AQ1" s="1">
         <v>99.8</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AR1" s="1">
         <v>99.83</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <v>-2</v>
       </c>
@@ -730,32 +746,38 @@
         <v>89.12</v>
       </c>
       <c r="P2" s="9">
+        <v>82.13</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>92.24</v>
+      </c>
+      <c r="R2" s="9">
         <v>50.23</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="S2" s="9">
         <v>57.25</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AB2" s="1">
         <v>1.0920000000000001E-2</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AC2" s="1">
         <v>1.8239999999999999E-2</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AD2" s="1">
         <v>97.25</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AE2" s="1">
         <v>95.11</v>
       </c>
-      <c r="AD2" s="8">
+      <c r="AF2" s="8">
         <v>92.58</v>
       </c>
-      <c r="AE2" s="1"/>
-      <c r="AJ2" s="1">
+      <c r="AG2" s="1"/>
+      <c r="AL2" s="1">
         <v>96.65</v>
       </c>
     </row>
-    <row r="3" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0.48799999999999999</v>
       </c>
@@ -802,64 +824,70 @@
         <v>93.45</v>
       </c>
       <c r="P3" s="2">
+        <v>89.24</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>94.56</v>
+      </c>
+      <c r="R3" s="2">
         <v>58.34</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="S3" s="2">
         <v>65.149999999999991</v>
       </c>
-      <c r="R3" s="2">
+      <c r="T3" s="2">
         <v>0.76959999999999995</v>
       </c>
-      <c r="S3" s="2">
+      <c r="U3" s="2">
         <v>0.83299999999999996</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <v>0.87219999999999998</v>
       </c>
-      <c r="U3" s="2">
+      <c r="W3" s="2">
         <v>0.83819999999999995</v>
       </c>
-      <c r="V3" s="2">
+      <c r="X3" s="2">
         <v>0.83640000000000003</v>
       </c>
-      <c r="W3" s="2">
+      <c r="Y3" s="2">
         <v>0.51385000000000003</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Z3" s="2">
         <v>0.26500000000000001</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="AA3" s="2">
         <v>-1</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AB3" s="2">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AC3" s="2">
         <v>1.52E-2</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AD3" s="2">
         <v>98.65</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AE3" s="2">
         <v>95.56</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AF3" s="8">
         <v>94.32</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AG3" s="2">
         <v>79.319999999999993</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AH3" s="2">
         <v>62.12</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AI3" s="2">
         <v>67.89</v>
       </c>
-      <c r="AJ3" s="2">
+      <c r="AL3" s="2">
         <v>98.48</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.38800000000000001</v>
       </c>
@@ -906,64 +934,70 @@
         <v>95.56</v>
       </c>
       <c r="P4" s="1">
+        <v>92.32</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>97.23</v>
+      </c>
+      <c r="R4" s="1">
         <v>65.75</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="S4" s="1">
         <v>70.45</v>
       </c>
-      <c r="R4" s="1">
+      <c r="T4" s="1">
         <v>0.85899999999999999</v>
       </c>
-      <c r="S4" s="1">
+      <c r="U4" s="1">
         <v>0.90059999999999996</v>
       </c>
-      <c r="T4" s="1">
+      <c r="V4" s="1">
         <v>0.90620000000000001</v>
       </c>
-      <c r="U4" s="1">
+      <c r="W4" s="1">
         <v>0.89180000000000004</v>
       </c>
-      <c r="V4" s="1">
+      <c r="X4" s="1">
         <v>0.86299999999999999</v>
       </c>
-      <c r="W4" s="1">
+      <c r="Y4" s="1">
         <v>0.4975</v>
       </c>
-      <c r="X4" s="1">
+      <c r="Z4" s="1">
         <v>0.21</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AA4" s="1">
         <v>0</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AB4" s="1">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AC4" s="1">
         <v>1.29E-2</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AD4" s="1">
         <v>99.25</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AE4" s="1">
         <v>96.47</v>
       </c>
-      <c r="AD4" s="8">
+      <c r="AF4" s="8">
         <v>95.67</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AG4" s="1">
         <v>81.41</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AH4" s="1">
         <v>67.11</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AI4" s="1">
         <v>73.56</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AL4" s="1">
         <v>99.23</v>
       </c>
     </row>
-    <row r="5" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0.308</v>
       </c>
@@ -1010,64 +1044,70 @@
         <v>96.34</v>
       </c>
       <c r="P5" s="2">
+        <v>93.56</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>97.86</v>
+      </c>
+      <c r="R5" s="2">
         <v>76.465000000000003</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="S5" s="2">
         <v>81.540000000000006</v>
       </c>
-      <c r="R5" s="2">
+      <c r="T5" s="2">
         <v>0.89159999999999995</v>
       </c>
-      <c r="S5" s="2">
+      <c r="U5" s="2">
         <v>0.91820000000000002</v>
       </c>
-      <c r="T5" s="2">
+      <c r="V5" s="2">
         <v>0.93840000000000001</v>
       </c>
-      <c r="U5" s="2">
+      <c r="W5" s="2">
         <v>0.9234</v>
       </c>
-      <c r="V5" s="2">
+      <c r="X5" s="2">
         <v>0.90059999999999996</v>
       </c>
-      <c r="W5" s="2">
+      <c r="Y5" s="2">
         <v>0.59560000000000002</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Z5" s="2">
         <v>0.16500000000000001</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="AA5" s="2">
         <v>1</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AB5" s="2">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AC5" s="2">
         <v>1.15E-2</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AD5" s="2">
         <v>99.39</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AE5" s="2">
         <v>97.58</v>
       </c>
-      <c r="AD5" s="8">
+      <c r="AF5" s="8">
         <v>96.87</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AG5" s="2">
         <v>87.92</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AH5" s="2">
         <v>77.239999999999995</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AI5" s="2">
         <v>83.45</v>
       </c>
-      <c r="AJ5" s="2">
+      <c r="AL5" s="2">
         <v>99.34</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.245</v>
       </c>
@@ -1114,64 +1154,70 @@
         <v>97.45</v>
       </c>
       <c r="P6" s="1">
+        <v>94.88</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>98.45</v>
+      </c>
+      <c r="R6" s="1">
         <v>79.135000000000005</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="S6" s="1">
         <v>82.64</v>
       </c>
-      <c r="R6" s="1">
+      <c r="T6" s="1">
         <v>0.93340000000000001</v>
       </c>
-      <c r="S6" s="1">
+      <c r="U6" s="1">
         <v>0.95540000000000003</v>
       </c>
-      <c r="T6" s="1">
+      <c r="V6" s="1">
         <v>0.97119999999999995</v>
       </c>
-      <c r="U6" s="1">
+      <c r="W6" s="1">
         <v>0.95320000000000005</v>
       </c>
-      <c r="V6" s="1">
+      <c r="X6" s="1">
         <v>0.93799999999999994</v>
       </c>
-      <c r="W6" s="1">
+      <c r="Y6" s="1">
         <v>0.74129999999999996</v>
       </c>
-      <c r="X6" s="1">
+      <c r="Z6" s="1">
         <v>0.13</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AA6" s="1">
         <v>2</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AB6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AC6" s="1">
         <v>1.06E-2</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AD6" s="1">
         <v>99.48</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AE6" s="1">
         <v>98.26</v>
       </c>
-      <c r="AD6" s="8">
+      <c r="AF6" s="8">
         <v>97.54</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AG6" s="1">
         <v>95.12</v>
       </c>
-      <c r="AF6" s="1">
+      <c r="AH6" s="1">
         <v>79.98</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AI6" s="1">
         <v>84.21</v>
       </c>
-      <c r="AJ6" s="1">
+      <c r="AL6" s="1">
         <v>99.42</v>
       </c>
     </row>
-    <row r="7" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0.19400000000000001</v>
       </c>
@@ -1218,64 +1264,70 @@
         <v>98.12</v>
       </c>
       <c r="P7" s="2">
+        <v>96.58</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>98.92</v>
+      </c>
+      <c r="R7" s="2">
         <v>79.650000000000006</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="S7" s="2">
         <v>84.56</v>
       </c>
-      <c r="R7" s="2">
+      <c r="T7" s="2">
         <v>0.9446</v>
       </c>
-      <c r="S7" s="2">
+      <c r="U7" s="2">
         <v>0.95960000000000001</v>
       </c>
-      <c r="T7" s="2">
+      <c r="V7" s="2">
         <v>0.97919999999999996</v>
       </c>
-      <c r="U7" s="2">
+      <c r="W7" s="2">
         <v>0.96099999999999997</v>
       </c>
-      <c r="V7" s="2">
+      <c r="X7" s="2">
         <v>0.95179999999999998</v>
       </c>
-      <c r="W7" s="2">
+      <c r="Y7" s="2">
         <v>0.90310000000000001</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Z7" s="2">
         <v>0.105</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="AA7" s="2">
         <v>3</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AB7" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AC7" s="2">
         <v>1.01E-2</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AD7" s="2">
         <v>99.53</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AE7" s="2">
         <v>98.56</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AF7" s="8">
         <v>98.12</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AG7" s="2">
         <v>95.78</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AH7" s="2">
         <v>81.150000000000006</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AI7" s="2">
         <v>86.32</v>
       </c>
-      <c r="AJ7" s="2">
+      <c r="AL7" s="2">
         <v>99.48</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.154</v>
       </c>
@@ -1322,64 +1374,70 @@
         <v>98.56</v>
       </c>
       <c r="P8" s="1">
+        <v>97.54</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>99.08</v>
+      </c>
+      <c r="R8" s="1">
         <v>79.959999999999994</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="S8" s="1">
         <v>86.74</v>
       </c>
-      <c r="R8" s="1">
+      <c r="T8" s="1">
         <v>0.97619999999999996</v>
       </c>
-      <c r="S8" s="1">
+      <c r="U8" s="1">
         <v>0.98119999999999996</v>
       </c>
-      <c r="T8" s="1">
+      <c r="V8" s="1">
         <v>0.99019999999999997</v>
       </c>
-      <c r="U8" s="1">
+      <c r="W8" s="1">
         <v>0.97860000000000003</v>
       </c>
-      <c r="V8" s="1">
+      <c r="X8" s="1">
         <v>0.96799999999999997</v>
       </c>
-      <c r="W8" s="1">
+      <c r="Y8" s="1">
         <v>0.95184999999999997</v>
       </c>
-      <c r="X8" s="1">
+      <c r="Z8" s="1">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AA8" s="1">
         <v>4</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="AB8" s="1">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AC8" s="1">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AD8" s="1">
         <v>99.67</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AE8" s="1">
         <v>98.78</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AF8" s="8">
         <v>98.42</v>
       </c>
-      <c r="AE8" s="1">
+      <c r="AG8" s="1">
         <v>96.54</v>
       </c>
-      <c r="AF8" s="1">
+      <c r="AH8" s="1">
         <v>81.14</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AI8" s="1">
         <v>88.45</v>
       </c>
-      <c r="AJ8" s="1">
+      <c r="AL8" s="1">
         <v>99.58</v>
       </c>
     </row>
-    <row r="9" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0.123</v>
       </c>
@@ -1426,64 +1484,70 @@
         <v>98.78</v>
       </c>
       <c r="P9" s="2">
+        <v>98.12</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>99.32</v>
+      </c>
+      <c r="R9" s="2">
         <v>82.34</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="S9" s="2">
         <v>88.38000000000001</v>
       </c>
-      <c r="R9" s="2">
+      <c r="T9" s="2">
         <v>0.97199999999999998</v>
       </c>
-      <c r="S9" s="2">
+      <c r="U9" s="2">
         <v>0.98160000000000003</v>
       </c>
-      <c r="T9" s="2">
+      <c r="V9" s="2">
         <v>0.99239999999999995</v>
       </c>
-      <c r="U9" s="2">
+      <c r="W9" s="2">
         <v>0.98340000000000005</v>
       </c>
-      <c r="V9" s="2">
+      <c r="X9" s="2">
         <v>0.98580000000000001</v>
       </c>
-      <c r="W9" s="2">
+      <c r="Y9" s="2">
         <v>0.96230000000000004</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Z9" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="AA9" s="2">
         <v>5</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AB9" s="2">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AC9" s="2">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AD9" s="2">
         <v>99.72</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AE9" s="2">
         <v>98.81</v>
       </c>
-      <c r="AD9" s="8">
+      <c r="AF9" s="8">
         <v>98.63</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AG9" s="2">
         <v>97.23</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="AH9" s="2">
         <v>83.24</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="AI9" s="2">
         <v>91.29</v>
       </c>
-      <c r="AJ9" s="2">
+      <c r="AL9" s="2">
         <v>99.6</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9.6000000000000002E-2</v>
       </c>
@@ -1530,64 +1594,70 @@
         <v>98.89</v>
       </c>
       <c r="P10" s="1">
+        <v>98.57</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>99.4</v>
+      </c>
+      <c r="R10" s="1">
         <v>83.12</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="S10" s="1">
         <v>90.259999999999991</v>
       </c>
-      <c r="R10" s="1">
+      <c r="T10" s="1">
         <v>0.97940000000000005</v>
       </c>
-      <c r="S10" s="1">
+      <c r="U10" s="1">
         <v>0.98480000000000001</v>
       </c>
-      <c r="T10" s="1">
+      <c r="V10" s="1">
         <v>0.99519999999999997</v>
       </c>
-      <c r="U10" s="1">
+      <c r="W10" s="1">
         <v>0.98899999999999999</v>
       </c>
-      <c r="V10" s="1">
+      <c r="X10" s="1">
         <v>0.99019999999999997</v>
       </c>
-      <c r="W10" s="1">
+      <c r="Y10" s="1">
         <v>0.97529999999999994</v>
       </c>
-      <c r="X10" s="1">
+      <c r="Z10" s="1">
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="AA10" s="1">
         <v>6</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AB10" s="1">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AC10" s="1">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AD10" s="2">
         <v>99.72</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AE10" s="1">
         <v>98.85</v>
       </c>
-      <c r="AD10" s="8">
+      <c r="AF10" s="8">
         <v>98.89</v>
       </c>
-      <c r="AE10" s="1">
+      <c r="AG10" s="1">
         <v>97.34</v>
       </c>
-      <c r="AF10" s="1">
+      <c r="AH10" s="1">
         <v>84.89</v>
       </c>
-      <c r="AG10" s="1">
+      <c r="AI10" s="1">
         <v>92.56</v>
       </c>
-      <c r="AJ10" s="1">
+      <c r="AL10" s="1">
         <v>99.63</v>
       </c>
     </row>
-    <row r="11" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>7.6999999999999999E-2</v>
       </c>
@@ -1634,64 +1704,70 @@
         <v>98.98</v>
       </c>
       <c r="P11" s="2">
+        <v>98.96</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>99.52</v>
+      </c>
+      <c r="R11" s="2">
         <v>83.45</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="S11" s="2">
         <v>91.05</v>
       </c>
-      <c r="R11" s="2">
+      <c r="T11" s="2">
         <v>0.98340000000000005</v>
       </c>
-      <c r="S11" s="2">
+      <c r="U11" s="2">
         <v>0.98919999999999997</v>
       </c>
-      <c r="T11" s="2">
+      <c r="V11" s="2">
         <v>0.99719999999999998</v>
       </c>
-      <c r="U11" s="2">
+      <c r="W11" s="2">
         <v>0.99560000000000004</v>
       </c>
-      <c r="V11" s="2">
+      <c r="X11" s="2">
         <v>0.99439999999999995</v>
       </c>
-      <c r="W11" s="2">
+      <c r="Y11" s="2">
         <v>0.9778</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Z11" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="AA11" s="2">
         <v>7</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="AB11" s="2">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="AA11" s="2">
+      <c r="AC11" s="2">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AD11" s="1">
         <v>99.75</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AE11" s="1">
         <v>98.87</v>
       </c>
-      <c r="AD11" s="8">
+      <c r="AF11" s="8">
         <v>99.08</v>
       </c>
-      <c r="AE11" s="2">
+      <c r="AG11" s="2">
         <v>97.36</v>
       </c>
-      <c r="AF11" s="2">
+      <c r="AH11" s="2">
         <v>85.45</v>
       </c>
-      <c r="AG11" s="2">
+      <c r="AI11" s="2">
         <v>92.87</v>
       </c>
-      <c r="AJ11" s="2">
+      <c r="AL11" s="2">
         <v>99.67</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>6.1499999999999999E-2</v>
       </c>
@@ -1738,64 +1814,70 @@
         <v>99.04</v>
       </c>
       <c r="P12" s="1">
+        <v>99.1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>99.64</v>
+      </c>
+      <c r="R12" s="1">
         <v>84.11999999999999</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="S12" s="1">
         <v>91.25</v>
       </c>
-      <c r="R12" s="1">
+      <c r="T12" s="1">
         <v>0.98740000000000006</v>
       </c>
-      <c r="S12" s="1">
+      <c r="U12" s="1">
         <v>0.99</v>
-      </c>
-      <c r="T12" s="1">
-        <v>0.997</v>
-      </c>
-      <c r="U12" s="1">
-        <v>0.99680000000000002</v>
       </c>
       <c r="V12" s="1">
         <v>0.997</v>
       </c>
       <c r="W12" s="1">
+        <v>0.99680000000000002</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0.997</v>
+      </c>
+      <c r="Y12" s="1">
         <v>0.97850000000000004</v>
       </c>
-      <c r="X12" s="1">
+      <c r="Z12" s="1">
         <v>3.2500000000000001E-2</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AA12" s="1">
         <v>8</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="AB12" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AC12" s="1">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AD12" s="2">
         <v>99.8</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AE12" s="1">
         <v>98.83</v>
       </c>
-      <c r="AD12" s="8">
+      <c r="AF12" s="8">
         <v>99.21</v>
       </c>
-      <c r="AE12" s="1">
+      <c r="AG12" s="1">
         <v>97.38</v>
       </c>
-      <c r="AF12" s="1">
+      <c r="AH12" s="1">
         <v>86.16</v>
       </c>
-      <c r="AG12" s="1">
+      <c r="AI12" s="1">
         <v>93.19</v>
       </c>
-      <c r="AJ12" s="1">
+      <c r="AL12" s="1">
         <v>99.72</v>
       </c>
     </row>
-    <row r="13" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>4.8500000000000001E-2</v>
       </c>
@@ -1842,64 +1924,70 @@
         <v>99.1</v>
       </c>
       <c r="P13" s="2">
+        <v>99.25</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>99.68</v>
+      </c>
+      <c r="R13" s="2">
         <v>84.31</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="S13" s="2">
         <v>92.45</v>
       </c>
-      <c r="R13" s="2">
+      <c r="T13" s="2">
         <v>0.98399999999999999</v>
       </c>
-      <c r="S13" s="2">
+      <c r="U13" s="2">
         <v>0.98860000000000003</v>
       </c>
-      <c r="T13" s="2">
+      <c r="V13" s="2">
         <v>0.997</v>
       </c>
-      <c r="U13" s="2">
+      <c r="W13" s="2">
         <v>0.995</v>
       </c>
-      <c r="V13" s="2">
+      <c r="X13" s="2">
         <v>0.99380000000000002</v>
       </c>
-      <c r="W13" s="2">
+      <c r="Y13" s="2">
         <v>0.97909999999999997</v>
       </c>
-      <c r="X13" s="2">
+      <c r="Z13" s="2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="AA13" s="2">
         <v>9</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AB13" s="2">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AC13" s="2">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AD13" s="2">
         <v>99.82</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AE13" s="2">
         <v>99.02</v>
       </c>
-      <c r="AD13" s="8">
+      <c r="AF13" s="8">
         <v>99.38</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AG13" s="2">
         <v>97.43</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="AH13" s="2">
         <v>86.45</v>
       </c>
-      <c r="AG13" s="2">
+      <c r="AI13" s="2">
         <v>93.45</v>
       </c>
-      <c r="AJ13" s="2">
+      <c r="AL13" s="2">
         <v>99.72</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>3.9E-2</v>
       </c>
@@ -1946,64 +2034,70 @@
         <v>99.16</v>
       </c>
       <c r="P14" s="1">
+        <v>99.46</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>99.7</v>
+      </c>
+      <c r="R14" s="1">
         <v>84.53</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="S14" s="1">
         <v>92.53</v>
       </c>
-      <c r="R14" s="1">
+      <c r="T14" s="1">
         <v>0.98740000000000006</v>
       </c>
-      <c r="S14" s="1">
+      <c r="U14" s="1">
         <v>0.99280000000000002</v>
       </c>
-      <c r="T14" s="1">
+      <c r="V14" s="1">
         <v>0.99639999999999995</v>
       </c>
-      <c r="U14" s="1">
+      <c r="W14" s="1">
         <v>0.99719999999999998</v>
       </c>
-      <c r="V14" s="1">
+      <c r="X14" s="1">
         <v>0.998</v>
       </c>
-      <c r="W14" s="1">
+      <c r="Y14" s="1">
         <v>0.98050000000000004</v>
       </c>
-      <c r="X14" s="1">
+      <c r="Z14" s="1">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="AA14" s="1">
         <v>10</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AB14" s="1">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="AA14" s="1">
+      <c r="AC14" s="1">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="AB14" s="1">
+      <c r="AD14" s="1">
         <v>99.85</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AE14" s="1">
         <v>99.1</v>
       </c>
-      <c r="AD14" s="8">
+      <c r="AF14" s="8">
         <v>99.52</v>
       </c>
-      <c r="AE14" s="1">
+      <c r="AG14" s="1">
         <v>97.56</v>
       </c>
-      <c r="AF14" s="1">
+      <c r="AH14" s="1">
         <v>86.78</v>
       </c>
-      <c r="AG14" s="1">
+      <c r="AI14" s="1">
         <v>93.89</v>
       </c>
-      <c r="AJ14" s="1">
+      <c r="AL14" s="1">
         <v>99.75</v>
       </c>
     </row>
-    <row r="15" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3.1E-2</v>
       </c>
@@ -2050,64 +2144,70 @@
         <v>99.2</v>
       </c>
       <c r="P15" s="2">
+        <v>99.54</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>99.72</v>
+      </c>
+      <c r="R15" s="2">
         <v>85.67</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="S15" s="2">
         <v>92.67</v>
       </c>
-      <c r="R15" s="2">
+      <c r="T15" s="2">
         <v>0.98480000000000001</v>
       </c>
-      <c r="S15" s="2">
+      <c r="U15" s="2">
         <v>0.99099999999999999</v>
       </c>
-      <c r="T15" s="2">
+      <c r="V15" s="2">
         <v>0.99680000000000002</v>
       </c>
-      <c r="U15" s="2">
+      <c r="W15" s="2">
         <v>0.99680000000000002</v>
       </c>
-      <c r="V15" s="2">
+      <c r="X15" s="2">
         <v>0.99819999999999998</v>
       </c>
-      <c r="W15" s="2">
+      <c r="Y15" s="2">
         <v>0.98165000000000002</v>
       </c>
-      <c r="X15" s="2">
+      <c r="Z15" s="2">
         <v>1.6500000000000001E-2</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="AA15" s="2">
         <v>11</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="AB15" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="AC15" s="2">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="AD15" s="2">
         <v>99.88</v>
       </c>
-      <c r="AC15" s="1">
+      <c r="AE15" s="1">
         <v>99.12</v>
       </c>
-      <c r="AD15" s="8">
+      <c r="AF15" s="8">
         <v>99.78</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="AG15" s="2">
         <v>97.59</v>
       </c>
-      <c r="AF15" s="2">
+      <c r="AH15" s="2">
         <v>87.12</v>
       </c>
-      <c r="AG15" s="2">
+      <c r="AI15" s="2">
         <v>94.12</v>
       </c>
-      <c r="AJ15" s="2">
+      <c r="AL15" s="2">
         <v>99.78</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2.4500000000000001E-2</v>
       </c>
@@ -2154,75 +2254,81 @@
         <v>99.24</v>
       </c>
       <c r="P16" s="1">
+        <v>99.69</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>99.75</v>
+      </c>
+      <c r="R16" s="1">
         <v>85.78</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="S16" s="1">
         <v>92.78</v>
       </c>
-      <c r="R16" s="1">
+      <c r="T16" s="1">
         <v>0.98899999999999999</v>
       </c>
-      <c r="S16" s="1">
+      <c r="U16" s="1">
         <v>0.99280000000000002</v>
       </c>
-      <c r="T16" s="1">
+      <c r="V16" s="1">
         <v>0.99780000000000002</v>
       </c>
-      <c r="U16" s="1">
+      <c r="W16" s="1">
         <v>0.99719999999999998</v>
       </c>
-      <c r="V16" s="1">
+      <c r="X16" s="1">
         <v>0.99760000000000004</v>
       </c>
-      <c r="W16" s="1">
+      <c r="Y16" s="1">
         <v>0.98124999999999996</v>
       </c>
-      <c r="X16" s="1">
+      <c r="Z16" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="AA16" s="1">
         <v>12</v>
       </c>
-      <c r="Z16" s="1">
+      <c r="AB16" s="1">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="AA16" s="1">
+      <c r="AC16" s="1">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="AB16" s="1">
+      <c r="AD16" s="1">
         <v>99.89</v>
       </c>
-      <c r="AC16" s="1">
+      <c r="AE16" s="1">
         <v>99.12</v>
       </c>
-      <c r="AD16" s="8">
+      <c r="AF16" s="8">
         <v>99.83</v>
       </c>
-      <c r="AE16" s="1">
+      <c r="AG16" s="1">
         <v>97.61</v>
       </c>
-      <c r="AF16" s="1">
+      <c r="AH16" s="1">
         <v>87.23</v>
       </c>
-      <c r="AG16" s="1">
+      <c r="AI16" s="1">
         <v>94.23</v>
       </c>
-      <c r="AJ16" s="1">
+      <c r="AL16" s="1">
         <v>99.78</v>
       </c>
     </row>
-    <row r="17" spans="4:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:39" x14ac:dyDescent="0.2">
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
-      <c r="AE17" s="12"/>
-    </row>
-    <row r="18" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="AG17" s="12"/>
+    </row>
+    <row r="18" spans="4:39" x14ac:dyDescent="0.2">
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="4"/>
-    </row>
-    <row r="19" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="AG18" s="13"/>
+      <c r="AH18" s="4"/>
+    </row>
+    <row r="19" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -2244,10 +2350,12 @@
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="AE19" s="8"/>
-      <c r="AF19" s="4"/>
-    </row>
-    <row r="20" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="4"/>
+    </row>
+    <row r="20" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -2269,10 +2377,12 @@
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
-      <c r="AE20" s="8"/>
-      <c r="AF20" s="4"/>
-    </row>
-    <row r="21" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="4"/>
+    </row>
+    <row r="21" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -2294,10 +2404,12 @@
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
-      <c r="AE21" s="8"/>
-      <c r="AF21" s="4"/>
-    </row>
-    <row r="22" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="4"/>
+    </row>
+    <row r="22" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2319,10 +2431,12 @@
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
-      <c r="AE22" s="8"/>
-      <c r="AF22" s="4"/>
-    </row>
-    <row r="23" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="4"/>
+    </row>
+    <row r="23" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D23" s="4"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
@@ -2344,10 +2458,12 @@
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
-      <c r="AE23" s="8"/>
-      <c r="AF23" s="4"/>
-    </row>
-    <row r="24" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="4"/>
+    </row>
+    <row r="24" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D24" s="4"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
@@ -2369,10 +2485,12 @@
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
-      <c r="AE24" s="8"/>
-      <c r="AF24" s="4"/>
-    </row>
-    <row r="25" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="4"/>
+    </row>
+    <row r="25" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D25" s="4"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
@@ -2387,17 +2505,19 @@
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="4"/>
-    </row>
-    <row r="26" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AG25" s="8"/>
+      <c r="AH25" s="4"/>
+    </row>
+    <row r="26" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D26" s="4"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -2412,39 +2532,20 @@
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
-      <c r="AD26" s="1">
-        <v>97.25</v>
-      </c>
-      <c r="AE26" s="1">
-        <v>99.25</v>
-      </c>
-      <c r="AF26" s="1">
-        <v>99.48</v>
-      </c>
-      <c r="AG26" s="1">
-        <v>99.67</v>
-      </c>
-      <c r="AH26" s="2">
-        <v>99.72</v>
-      </c>
-      <c r="AI26" s="2">
-        <v>99.8</v>
-      </c>
-      <c r="AJ26" s="1">
-        <v>99.85</v>
-      </c>
-      <c r="AK26" s="1">
-        <v>99.89</v>
-      </c>
-    </row>
-    <row r="27" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AG26" s="1"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+    </row>
+    <row r="27" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2459,39 +2560,18 @@
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
-      <c r="AD27" s="1">
-        <v>95.11</v>
-      </c>
-      <c r="AE27" s="1">
-        <v>96.47</v>
-      </c>
-      <c r="AF27" s="1">
-        <v>98.26</v>
-      </c>
-      <c r="AG27" s="1">
-        <v>98.78</v>
-      </c>
-      <c r="AH27" s="1">
-        <v>98.85</v>
-      </c>
-      <c r="AI27" s="1">
-        <v>98.83</v>
-      </c>
-      <c r="AJ27" s="1">
-        <v>99.1</v>
-      </c>
-      <c r="AK27" s="1">
-        <v>99.12</v>
-      </c>
-    </row>
-    <row r="28" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AG27" s="1"/>
+    </row>
+    <row r="28" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2513,32 +2593,18 @@
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
-      <c r="AD28" s="8">
-        <v>92.58</v>
-      </c>
-      <c r="AE28" s="8">
-        <v>95.67</v>
-      </c>
-      <c r="AF28" s="8">
-        <v>97.54</v>
-      </c>
-      <c r="AG28" s="8">
-        <v>98.42</v>
-      </c>
-      <c r="AH28" s="8">
-        <v>98.89</v>
-      </c>
-      <c r="AI28" s="8">
-        <v>99.21</v>
-      </c>
-      <c r="AJ28" s="8">
-        <v>99.52</v>
-      </c>
-      <c r="AK28" s="8">
-        <v>99.83</v>
-      </c>
-    </row>
-    <row r="29" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AF28" s="8"/>
+      <c r="AG28" s="8"/>
+      <c r="AH28" s="8"/>
+      <c r="AI28" s="8"/>
+      <c r="AJ28" s="8"/>
+      <c r="AK28" s="8"/>
+      <c r="AL28" s="8"/>
+      <c r="AM28" s="8"/>
+    </row>
+    <row r="29" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2560,10 +2626,12 @@
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
-      <c r="AE29" s="8"/>
-      <c r="AF29" s="4"/>
-    </row>
-    <row r="30" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AG29" s="8"/>
+      <c r="AH29" s="4"/>
+    </row>
+    <row r="30" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2585,10 +2653,12 @@
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
-      <c r="AE30" s="8"/>
-      <c r="AF30" s="4"/>
-    </row>
-    <row r="31" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AG30" s="8"/>
+      <c r="AH30" s="4"/>
+    </row>
+    <row r="31" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2610,10 +2680,12 @@
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
-      <c r="AE31" s="8"/>
-      <c r="AF31" s="4"/>
-    </row>
-    <row r="32" spans="4:37" x14ac:dyDescent="0.2">
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
+      <c r="AG31" s="8"/>
+      <c r="AH31" s="4"/>
+    </row>
+    <row r="32" spans="4:39" x14ac:dyDescent="0.2">
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2635,10 +2707,12 @@
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
-      <c r="AE32" s="8"/>
-      <c r="AF32" s="4"/>
-    </row>
-    <row r="33" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="Y32" s="4"/>
+      <c r="Z32" s="4"/>
+      <c r="AG32" s="8"/>
+      <c r="AH32" s="4"/>
+    </row>
+    <row r="33" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2660,10 +2734,12 @@
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
       <c r="X33" s="4"/>
-      <c r="AE33" s="8"/>
-      <c r="AF33" s="4"/>
-    </row>
-    <row r="34" spans="4:32" x14ac:dyDescent="0.2">
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AG33" s="8"/>
+      <c r="AH33" s="4"/>
+    </row>
+    <row r="34" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2675,7 +2751,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2687,7 +2763,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2699,7 +2775,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -2711,7 +2787,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="4:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>

</xml_diff>